<commit_message>
using opencv for template matching
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\captaintsubasapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11145DD6-76F2-4DE9-B293-34C24FC0C9E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47F870C-8C43-4F1B-962B-DFC63E59CDE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{A635938C-4B30-4746-98CA-71BF6C54D22C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A635938C-4B30-4746-98CA-71BF6C54D22C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>001</t>
   </si>
@@ -49,14 +50,58 @@
   </si>
   <si>
     <t>Y End</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Run App</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>Enter App</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>Go to Story Mode</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>Go to Story Mode - Second Page</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>Middle School Part 1/3</t>
+  </si>
+  <si>
+    <t>Location X</t>
+  </si>
+  <si>
+    <t>Location Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,12 +129,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -406,57 +457,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D78686-76C6-452F-B587-8CDB6FAFC23B}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5234375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.7890625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.7890625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.05078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15" style="2" customWidth="1"/>
+    <col min="6" max="6" width="62.21875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>751</v>
+        <v>314</v>
       </c>
       <c r="C2" s="2">
-        <v>1003</v>
+        <v>141</v>
       </c>
       <c r="D2" s="2">
-        <v>969</v>
+        <v>467</v>
       </c>
       <c r="E2" s="2">
-        <v>1208</v>
+        <v>303</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2">
+        <v>690</v>
+      </c>
+      <c r="C3" s="2">
+        <v>479</v>
+      </c>
+      <c r="D3" s="2">
+        <v>891</v>
+      </c>
+      <c r="E3" s="2">
+        <v>631</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1029</v>
+      </c>
+      <c r="C4" s="2">
+        <v>465</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1423</v>
+      </c>
+      <c r="E4" s="2">
+        <v>565</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2">
+        <v>203</v>
+      </c>
+      <c r="C5" s="2">
+        <v>726</v>
+      </c>
+      <c r="D5" s="2">
+        <v>499</v>
+      </c>
+      <c r="E5" s="2">
+        <v>822</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
+        <v>227</v>
+      </c>
+      <c r="C6" s="2">
+        <v>306</v>
+      </c>
+      <c r="D6" s="2">
+        <v>525</v>
+      </c>
+      <c r="E6" s="2">
+        <v>502</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F41B98D-7245-4789-959E-C9764765CCC5}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
the app is ready next is to complete templates
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\captaintsubasapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B93EBF-E0D3-4A41-B324-3CDE12C357BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E78917-4192-440B-B333-3360387F3BD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A635938C-4B30-4746-98CA-71BF6C54D22C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>001</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>select friend</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>kick off button</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>go to scenario list</t>
   </si>
 </sst>
 </file>
@@ -493,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D78686-76C6-452F-B587-8CDB6FAFC23B}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,6 +739,46 @@
       </c>
       <c r="F11" s="2" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1344</v>
+      </c>
+      <c r="C12" s="2">
+        <v>729</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1717</v>
+      </c>
+      <c r="E12" s="2">
+        <v>829</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="2">
+        <v>746</v>
+      </c>
+      <c r="C13" s="2">
+        <v>924</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1092</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1012</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wait to recover energy
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\captaintsubasapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E78917-4192-440B-B333-3360387F3BD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62FF12D-C19F-407A-9958-79422A5CB1DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A635938C-4B30-4746-98CA-71BF6C54D22C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>001</t>
   </si>
@@ -134,6 +134,42 @@
   </si>
   <si>
     <t>go to scenario list</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>after match - you win</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>after match - break down</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>after match - rank up</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>recover energy - restore button</t>
+  </si>
+  <si>
+    <t>recover energy - cancel button</t>
+  </si>
+  <si>
+    <t>recover energy title</t>
   </si>
 </sst>
 </file>
@@ -505,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D78686-76C6-452F-B587-8CDB6FAFC23B}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -779,6 +815,126 @@
       </c>
       <c r="F13" s="2" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2">
+        <v>804</v>
+      </c>
+      <c r="C14" s="2">
+        <v>571</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1040</v>
+      </c>
+      <c r="E14" s="2">
+        <v>703</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="2">
+        <v>994</v>
+      </c>
+      <c r="C15" s="2">
+        <v>594</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1167</v>
+      </c>
+      <c r="E15" s="2">
+        <v>682</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2">
+        <v>656</v>
+      </c>
+      <c r="C16" s="2">
+        <v>488</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1191</v>
+      </c>
+      <c r="E16" s="2">
+        <v>589</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="2">
+        <v>716</v>
+      </c>
+      <c r="C17" s="2">
+        <v>147</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1124</v>
+      </c>
+      <c r="E17" s="2">
+        <v>223</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="2">
+        <v>639</v>
+      </c>
+      <c r="C18" s="2">
+        <v>826</v>
+      </c>
+      <c r="D18" s="2">
+        <v>823</v>
+      </c>
+      <c r="E18" s="2">
+        <v>901</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1012</v>
+      </c>
+      <c r="C19" s="2">
+        <v>827</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1204</v>
+      </c>
+      <c r="E19" s="2">
+        <v>902</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solo implemented club shared implemented new locator with imshow and many more ...
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,21 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\captaintsubasapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367BAFD1-85AA-4358-A5AC-55DAD156C94E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDE83DC-AE38-42BC-B484-7A79A8F74964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Templates" sheetId="1" r:id="rId1"/>
     <sheet name="Points" sheetId="2" r:id="rId2"/>
-    <sheet name="OCR" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
   <si>
     <t>Template Number</t>
   </si>
@@ -81,7 +80,7 @@
     <t>007</t>
   </si>
   <si>
-    <t>difficulty -&gt; very hard</t>
+    <t>difficulty -&gt; very hard horizontal</t>
   </si>
   <si>
     <t>008</t>
@@ -189,7 +188,7 @@
     <t>025</t>
   </si>
   <si>
-    <t>difficulty -&gt; extreme</t>
+    <t>difficulty -&gt; extreme horizontal</t>
   </si>
   <si>
     <t>026</t>
@@ -220,6 +219,54 @@
   </si>
   <si>
     <t>energy recovered dialog -&gt;  ok button</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">difficulty -&gt; very hard vertical </t>
+  </si>
+  <si>
+    <t>032</t>
+  </si>
+  <si>
+    <t>club shared playe button</t>
+  </si>
+  <si>
+    <t>033</t>
+  </si>
+  <si>
+    <t>club shared play - accepting member list -&gt; rank</t>
+  </si>
+  <si>
+    <t>034</t>
+  </si>
+  <si>
+    <t>join button</t>
+  </si>
+  <si>
+    <t>035</t>
+  </si>
+  <si>
+    <t>club shared play - accepting member list title</t>
+  </si>
+  <si>
+    <t>036</t>
+  </si>
+  <si>
+    <t>failed to join dialog -&gt; title</t>
+  </si>
+  <si>
+    <t>037</t>
+  </si>
+  <si>
+    <t>failed to join dialog -&gt; ok button</t>
+  </si>
+  <si>
+    <t>038</t>
+  </si>
+  <si>
+    <t>go to scenario list -&gt;  shared play</t>
   </si>
   <si>
     <t>Location Number</t>
@@ -603,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F39" sqref="A1:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,8 +664,8 @@
     <col min="4" max="4" width="13.77734375" style="2" customWidth="1"/>
     <col min="5" max="5" width="15" style="2" customWidth="1"/>
     <col min="6" max="6" width="62.21875" style="2" customWidth="1"/>
-    <col min="7" max="12" width="8.88671875" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="2"/>
+    <col min="7" max="17" width="8.88671875" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -686,16 +733,16 @@
         <v>10</v>
       </c>
       <c r="B4" s="2">
-        <v>1046</v>
+        <v>1082</v>
       </c>
       <c r="C4" s="2">
-        <v>483</v>
+        <v>235</v>
       </c>
       <c r="D4" s="2">
-        <v>1403</v>
+        <v>1410</v>
       </c>
       <c r="E4" s="2">
-        <v>538</v>
+        <v>288</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>11</v>
@@ -1239,6 +1286,166 @@
       </c>
       <c r="F31" s="2" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="2">
+        <v>696</v>
+      </c>
+      <c r="C32" s="2">
+        <v>269</v>
+      </c>
+      <c r="D32" s="2">
+        <v>810</v>
+      </c>
+      <c r="E32" s="2">
+        <v>350</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1550</v>
+      </c>
+      <c r="C33" s="2">
+        <v>926</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1683</v>
+      </c>
+      <c r="E33" s="2">
+        <v>1015</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="2">
+        <v>330</v>
+      </c>
+      <c r="C34" s="2">
+        <v>187</v>
+      </c>
+      <c r="D34" s="2">
+        <v>441</v>
+      </c>
+      <c r="E34" s="2">
+        <v>260</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1444</v>
+      </c>
+      <c r="C35" s="2">
+        <v>735</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1585</v>
+      </c>
+      <c r="E35" s="2">
+        <v>808</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="2">
+        <v>92</v>
+      </c>
+      <c r="C36" s="2">
+        <v>66</v>
+      </c>
+      <c r="D36" s="2">
+        <v>603</v>
+      </c>
+      <c r="E36" s="2">
+        <v>109</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="2">
+        <v>769</v>
+      </c>
+      <c r="C37" s="2">
+        <v>327</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1089</v>
+      </c>
+      <c r="E37" s="2">
+        <v>371</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="2">
+        <v>877</v>
+      </c>
+      <c r="C38" s="2">
+        <v>677</v>
+      </c>
+      <c r="D38" s="2">
+        <v>975</v>
+      </c>
+      <c r="E38" s="2">
+        <v>724</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="2">
+        <v>767</v>
+      </c>
+      <c r="C39" s="2">
+        <v>952</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1078</v>
+      </c>
+      <c r="E39" s="2">
+        <v>999</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1251,8 +1458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1265,13 +1472,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>5</v>
@@ -1288,23 +1495,11 @@
         <v>889</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add the ability to use one template with several positions add template 039
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\captaintsubasapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35060CBA-D448-4D5D-AED9-35F70B406771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA35EF9-E0CE-4922-B2C3-DE65E247379C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="89">
   <si>
     <t>Template Number</t>
   </si>
@@ -285,13 +285,16 @@
   </si>
   <si>
     <t xml:space="preserve">difficulty -&gt; normal vertical </t>
+  </si>
+  <si>
+    <t>File Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +306,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -656,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,12 +678,13 @@
     <col min="3" max="3" width="14.77734375" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" style="2" customWidth="1"/>
     <col min="5" max="5" width="15" style="2" customWidth="1"/>
-    <col min="6" max="6" width="62.21875" style="2" customWidth="1"/>
-    <col min="7" max="17" width="8.88671875" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="2"/>
+    <col min="6" max="6" width="15" style="1" customWidth="1"/>
+    <col min="7" max="7" width="62.21875" style="2" customWidth="1"/>
+    <col min="8" max="18" width="8.88671875" style="2" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -690,11 +700,14 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -710,11 +723,14 @@
       <c r="E2" s="2">
         <v>365</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -730,11 +746,14 @@
       <c r="E3" s="2">
         <v>571</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -750,11 +769,14 @@
       <c r="E4" s="2">
         <v>288</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -770,11 +792,14 @@
       <c r="E5" s="2">
         <v>794</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -790,11 +815,14 @@
       <c r="E6" s="2">
         <v>417</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -810,11 +838,14 @@
       <c r="E7" s="2">
         <v>592</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -830,11 +861,14 @@
       <c r="E8" s="2">
         <v>314</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -850,11 +884,14 @@
       <c r="E9" s="2">
         <v>889</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -870,11 +907,14 @@
       <c r="E10" s="2">
         <v>620</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -890,11 +930,14 @@
       <c r="E11" s="2">
         <v>416</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -910,11 +953,14 @@
       <c r="E12" s="2">
         <v>806</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -930,11 +976,14 @@
       <c r="E13" s="2">
         <v>995</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -950,11 +999,14 @@
       <c r="E14" s="2">
         <v>685</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -970,11 +1022,14 @@
       <c r="E15" s="2">
         <v>682</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -990,11 +1045,14 @@
       <c r="E16" s="2">
         <v>589</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1010,11 +1068,14 @@
       <c r="E17" s="2">
         <v>222</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
@@ -1030,11 +1091,14 @@
       <c r="E18" s="2">
         <v>900</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
@@ -1050,11 +1114,14 @@
       <c r="E19" s="2">
         <v>901</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
@@ -1070,11 +1137,14 @@
       <c r="E20" s="2">
         <v>251</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -1090,11 +1160,14 @@
       <c r="E21" s="2">
         <v>952</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
@@ -1110,11 +1183,14 @@
       <c r="E22" s="2">
         <v>381</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>48</v>
       </c>
@@ -1130,11 +1206,14 @@
       <c r="E23" s="2">
         <v>738</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
@@ -1150,11 +1229,14 @@
       <c r="E24" s="2">
         <v>477</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
@@ -1170,11 +1252,14 @@
       <c r="E25" s="2">
         <v>545</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -1190,11 +1275,14 @@
       <c r="E26" s="2">
         <v>349</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
@@ -1210,11 +1298,14 @@
       <c r="E27" s="2">
         <v>748</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>58</v>
       </c>
@@ -1230,11 +1321,14 @@
       <c r="E28" s="2">
         <v>161</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>60</v>
       </c>
@@ -1250,11 +1344,14 @@
       <c r="E29" s="2">
         <v>927</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>62</v>
       </c>
@@ -1270,11 +1367,14 @@
       <c r="E30" s="2">
         <v>374</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>64</v>
       </c>
@@ -1290,11 +1390,14 @@
       <c r="E31" s="2">
         <v>736</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>66</v>
       </c>
@@ -1310,11 +1413,14 @@
       <c r="E32" s="2">
         <v>350</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>68</v>
       </c>
@@ -1330,11 +1436,14 @@
       <c r="E33" s="2">
         <v>1015</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>70</v>
       </c>
@@ -1350,11 +1459,14 @@
       <c r="E34" s="2">
         <v>260</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
@@ -1370,11 +1482,14 @@
       <c r="E35" s="2">
         <v>808</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>74</v>
       </c>
@@ -1390,11 +1505,14 @@
       <c r="E36" s="2">
         <v>109</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>76</v>
       </c>
@@ -1410,11 +1528,14 @@
       <c r="E37" s="2">
         <v>371</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>78</v>
       </c>
@@ -1430,11 +1551,14 @@
       <c r="E38" s="2">
         <v>724</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
@@ -1450,11 +1574,14 @@
       <c r="E39" s="2">
         <v>1003</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>86</v>
       </c>
@@ -1470,11 +1597,15 @@
       <c r="E40" s="2">
         <v>327</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update 038 update 012
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\captaintsubasapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D230B8-E08B-4998-A119-72243659D91B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7D9F3B-EC42-4CA4-909C-9E6133435A52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -965,16 +965,16 @@
         <v>28</v>
       </c>
       <c r="B13" s="2">
-        <v>755</v>
+        <v>858</v>
       </c>
       <c r="C13" s="2">
-        <v>946</v>
+        <v>954</v>
       </c>
       <c r="D13" s="2">
-        <v>1085</v>
+        <v>1007</v>
       </c>
       <c r="E13" s="2">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>28</v>
@@ -1563,19 +1563,19 @@
         <v>80</v>
       </c>
       <c r="B39" s="2">
-        <v>755</v>
+        <v>858</v>
       </c>
       <c r="C39" s="2">
-        <v>950</v>
+        <v>954</v>
       </c>
       <c r="D39" s="2">
-        <v>1085</v>
+        <v>1007</v>
       </c>
       <c r="E39" s="2">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
new templates : 047, 048, 049
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\captaintsubasapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DED979-DE23-40FF-B2EB-BB5A7D206C39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86B0181-E3C5-49F1-83A1-8040237D135F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="109">
   <si>
     <t>Template Number</t>
   </si>
@@ -324,6 +324,30 @@
   </si>
   <si>
     <t>solo play - global disabled</t>
+  </si>
+  <si>
+    <t>046</t>
+  </si>
+  <si>
+    <t>047</t>
+  </si>
+  <si>
+    <t>048</t>
+  </si>
+  <si>
+    <t>049</t>
+  </si>
+  <si>
+    <t>ok button - unable to play dialog</t>
+  </si>
+  <si>
+    <t>unable to play dialog - max number of player -&gt; join</t>
+  </si>
+  <si>
+    <t>match condition have not met dialog - join</t>
+  </si>
+  <si>
+    <t>close button - match condition have not met dialog</t>
   </si>
 </sst>
 </file>
@@ -701,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1776,6 +1800,98 @@
       </c>
       <c r="G46" s="2" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" s="2">
+        <v>386</v>
+      </c>
+      <c r="C47" s="2">
+        <v>466</v>
+      </c>
+      <c r="D47" s="2">
+        <v>684</v>
+      </c>
+      <c r="E47" s="2">
+        <v>524</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" s="2">
+        <v>886</v>
+      </c>
+      <c r="C48" s="2">
+        <v>681</v>
+      </c>
+      <c r="D48" s="2">
+        <v>960</v>
+      </c>
+      <c r="E48" s="2">
+        <v>723</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="2">
+        <v>495</v>
+      </c>
+      <c r="C49" s="2">
+        <v>152</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1342</v>
+      </c>
+      <c r="E49" s="2">
+        <v>196</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" s="2">
+        <v>463</v>
+      </c>
+      <c r="C50" s="2">
+        <v>826</v>
+      </c>
+      <c r="D50" s="2">
+        <v>615</v>
+      </c>
+      <c r="E50" s="2">
+        <v>893</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed 053 fix run_033
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\captaintsubasapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF625AEF-2B20-4317-82AC-71AAB090601C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D0C057-9EFA-4E8C-99AB-348DAC63706A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="115">
   <si>
     <t>Template Number</t>
   </si>
@@ -365,13 +365,7 @@
     <t>052</t>
   </si>
   <si>
-    <t>053</t>
-  </si>
-  <si>
     <t>connection error dialog -&gt; shared</t>
-  </si>
-  <si>
-    <t>ok button - connection error dialog</t>
   </si>
 </sst>
 </file>
@@ -749,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1984,30 +1978,7 @@
         <v>113</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="B54" s="2">
-        <v>877</v>
-      </c>
-      <c r="C54" s="2">
-        <v>677</v>
-      </c>
-      <c r="D54" s="2">
-        <v>975</v>
-      </c>
-      <c r="E54" s="2">
-        <v>724</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
run 057 automatically based on config
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1960,16 +1960,16 @@
         </is>
       </c>
       <c r="B54" s="5" t="n">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="C54" s="5" t="n">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D54" s="5" t="n">
-        <v>800</v>
+        <v>836</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F54" s="8" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
update for ramadan event
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1078,16 +1078,16 @@
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>464</v>
+        <v>486</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>362</v>
+        <v>302</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="F24" s="1" t="inlineStr">
         <is>
@@ -2035,16 +2035,16 @@
         </is>
       </c>
       <c r="B57" s="2" t="n">
-        <v>718</v>
+        <v>1546</v>
       </c>
       <c r="C57" s="2" t="n">
-        <v>243</v>
+        <v>280</v>
       </c>
       <c r="D57" s="2" t="n">
-        <v>832</v>
+        <v>1647</v>
       </c>
       <c r="E57" s="2" t="n">
-        <v>290</v>
+        <v>322</v>
       </c>
       <c r="F57" s="1" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
fix for Ramadan event
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\captaintsubasapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3B8FAE-15EE-4D06-8BCD-E850389B10EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95D1401-01A4-438A-A9A1-951FB4EF16E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="127">
   <si>
     <t>Template Number</t>
   </si>
@@ -384,6 +384,12 @@
   </si>
   <si>
     <t>event match -&gt; to event exchange shop</t>
+  </si>
+  <si>
+    <t>062</t>
+  </si>
+  <si>
+    <t>after match -&gt; shared play reward</t>
   </si>
   <si>
     <t>Location Number</t>
@@ -767,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C51" sqref="A1:G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,8 +788,8 @@
     <col min="5" max="5" width="15" style="2" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" customWidth="1"/>
     <col min="7" max="7" width="62.21875" style="2" customWidth="1"/>
-    <col min="8" max="25" width="8.88671875" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="8.88671875" style="2"/>
+    <col min="8" max="26" width="8.88671875" style="2" customWidth="1"/>
+    <col min="27" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2118,6 +2124,29 @@
       </c>
       <c r="G58" s="2" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B59" s="2">
+        <v>772</v>
+      </c>
+      <c r="C59" s="2">
+        <v>107</v>
+      </c>
+      <c r="D59" s="2">
+        <v>1077</v>
+      </c>
+      <c r="E59" s="2">
+        <v>146</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2144,13 +2173,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>6</v>
@@ -2167,7 +2196,7 @@
         <v>889</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
detect inactive users in shared game play
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\captaintsubasapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD993FC3-A6B2-4CA3-93D0-6ADAA96057C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7AEECC-6FEB-4FF5-9388-DD3D892FFB93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="158">
   <si>
     <t>Template Number</t>
   </si>
@@ -462,6 +462,24 @@
   </si>
   <si>
     <t>home</t>
+  </si>
+  <si>
+    <t>075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shared play - preparing </t>
+  </si>
+  <si>
+    <t>076</t>
+  </si>
+  <si>
+    <t>confirm cancel dialog - title</t>
+  </si>
+  <si>
+    <t>077</t>
+  </si>
+  <si>
+    <t>confirm cancel dialog - ok button</t>
   </si>
   <si>
     <t>Location Number</t>
@@ -848,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="M61" sqref="M61"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C66" sqref="A1:G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,8 +881,8 @@
     <col min="5" max="5" width="15" style="4" customWidth="1"/>
     <col min="6" max="6" width="15" style="3" customWidth="1"/>
     <col min="7" max="7" width="62.21875" style="4" customWidth="1"/>
-    <col min="8" max="39" width="8.88671875" style="4" customWidth="1"/>
-    <col min="40" max="16384" width="8.88671875" style="4"/>
+    <col min="8" max="40" width="8.88671875" style="4" customWidth="1"/>
+    <col min="41" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2498,6 +2516,75 @@
       </c>
       <c r="G71" s="4" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B72" s="4">
+        <v>1273</v>
+      </c>
+      <c r="C72" s="4">
+        <v>838</v>
+      </c>
+      <c r="D72" s="4">
+        <v>1518</v>
+      </c>
+      <c r="E72" s="4">
+        <v>903</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B73" s="4">
+        <v>743</v>
+      </c>
+      <c r="C73" s="4">
+        <v>321</v>
+      </c>
+      <c r="D73" s="4">
+        <v>1103</v>
+      </c>
+      <c r="E73" s="4">
+        <v>373</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B74" s="4">
+        <v>1080</v>
+      </c>
+      <c r="C74" s="4">
+        <v>678</v>
+      </c>
+      <c r="D74" s="4">
+        <v>1178</v>
+      </c>
+      <c r="E74" s="4">
+        <v>725</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2524,13 +2611,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -2547,7 +2634,7 @@
         <v>889</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2561,7 +2648,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on league mode
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\captaintsubasapy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17538F44-250D-45F3-BA9C-27186FC575E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EC77E5-5AC9-494A-8921-FD4C3E5FEA01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="216">
   <si>
     <t>Template Number</t>
   </si>
@@ -636,6 +636,24 @@
   </si>
   <si>
     <t>total power -&gt; league mode -&gt; team select</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>half time stamina recovery +30% -&gt; league mode</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>stamina consumed -20% -&gt; league mode</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>kick off -&gt; league mode</t>
   </si>
   <si>
     <t>Location Number</t>
@@ -1022,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C99" sqref="A1:G101"/>
+      <selection activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1037,8 +1055,8 @@
     <col min="5" max="5" width="15" style="4" customWidth="1"/>
     <col min="6" max="6" width="15" style="3" customWidth="1"/>
     <col min="7" max="7" width="62.21875" style="4" customWidth="1"/>
-    <col min="8" max="74" width="8.88671875" style="4" customWidth="1"/>
-    <col min="75" max="16384" width="8.88671875" style="4"/>
+    <col min="8" max="75" width="8.88671875" style="4" customWidth="1"/>
+    <col min="76" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -3364,9 +3382,78 @@
         <v>204</v>
       </c>
     </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A102" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B102" s="4">
+        <v>368</v>
+      </c>
+      <c r="C102" s="4">
+        <v>736</v>
+      </c>
+      <c r="D102" s="4">
+        <v>504</v>
+      </c>
+      <c r="E102" s="4">
+        <v>856</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A103" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B103" s="4">
+        <v>718</v>
+      </c>
+      <c r="C103" s="4">
+        <v>736</v>
+      </c>
+      <c r="D103" s="4">
+        <v>854</v>
+      </c>
+      <c r="E103" s="4">
+        <v>856</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A104" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B104" s="4">
+        <v>1357</v>
+      </c>
+      <c r="C104" s="4">
+        <v>718</v>
+      </c>
+      <c r="D104" s="4">
+        <v>1708</v>
+      </c>
+      <c r="E104" s="4">
+        <v>828</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3388,13 +3475,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -3411,7 +3498,7 @@
         <v>889</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3425,7 +3512,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
you have already watched this story dialog
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -377,10 +377,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+      <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -391,8 +391,8 @@
     <col width="13.77734375" customWidth="1" style="4" min="4" max="4"/>
     <col width="15" customWidth="1" style="4" min="5" max="5"/>
     <col width="62.21875" customWidth="1" style="4" min="6" max="6"/>
-    <col width="8.88671875" customWidth="1" style="4" min="7" max="84"/>
-    <col width="8.88671875" customWidth="1" style="4" min="85" max="16384"/>
+    <col width="8.88671875" customWidth="1" style="4" min="7" max="85"/>
+    <col width="8.88671875" customWidth="1" style="4" min="86" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3304,6 +3304,54 @@
       <c r="F121" s="4" t="inlineStr">
         <is>
           <t>ok button in do you want to try again dialog in banner</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="3" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>501</v>
+      </c>
+      <c r="C122" t="n">
+        <v>322</v>
+      </c>
+      <c r="D122" t="n">
+        <v>1349</v>
+      </c>
+      <c r="E122" t="n">
+        <v>370</v>
+      </c>
+      <c r="F122" s="4" t="inlineStr">
+        <is>
+          <t>you have already watched this story dialog -&gt; title</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="3" t="inlineStr">
+        <is>
+          <t>126</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>631</v>
+      </c>
+      <c r="C123" t="n">
+        <v>680</v>
+      </c>
+      <c r="D123" t="n">
+        <v>809</v>
+      </c>
+      <c r="E123" t="n">
+        <v>728</v>
+      </c>
+      <c r="F123" s="4" t="inlineStr">
+        <is>
+          <t>you have already watched this story dialog -&gt; cancel button</t>
         </is>
       </c>
     </row>

</xml_diff>